<commit_message>
More examples and edits - updated for multiple questions
</commit_message>
<xml_diff>
--- a/data-raw/helena/Example Feedback.xlsx
+++ b/data-raw/helena/Example Feedback.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/NO NAME/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
@@ -16,11 +11,11 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -188,7 +183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -223,7 +218,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -400,7 +395,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -410,9 +405,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
@@ -425,7 +422,7 @@
     <col min="10" max="10" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +454,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="137" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="137" customHeight="1">
       <c r="A2">
         <v>12</v>
       </c>
@@ -491,5 +488,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>